<commit_message>
add new model + dbclasses
</commit_message>
<xml_diff>
--- a/RESTful_DBAccessMethods.xlsx
+++ b/RESTful_DBAccessMethods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20339"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKSPACE\repos\PROJ\Travel-Experts-Sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKSPACE\repos\_PROJ\Travel-Experts-Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF777EB-BBFC-4F22-B5AC-24228A866FF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B1532A-3B1D-4E7F-882B-EB1470B05A68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29130" yWindow="120" windowWidth="26730" windowHeight="15750" xr2:uid="{FAF48CAF-0C36-48CA-BE81-D54EEE776538}"/>
   </bookViews>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -682,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>